<commit_message>
done 4 exrcises from w6d1
</commit_message>
<xml_diff>
--- a/Week6/Day1/ExerciseXP/List of Holidays(ex2).xlsx
+++ b/Week6/Day1/ExerciseXP/List of Holidays(ex2).xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margotiamanova/Desktop/DI-Bootcamp/Week6/Day1/ExerciseXP/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{406C33DF-49E4-DF4E-83AC-E530CA5D4D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="16215" windowHeight="8415"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Source Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Source Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
     <t>Wise Owl Travel Agents</t>
   </si>
@@ -215,16 +225,28 @@
   </si>
   <si>
     <t>SV767HH</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(Multiple Items)</t>
+  </si>
+  <si>
+    <t>Average of Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -312,17 +334,518 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="1"/>
+    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45732.617139236114" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="28" xr:uid="{41A770B7-7608-F040-9D91-4C7F751B01A1}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A3:F31" sheet="Source Data"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Country" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Resort Name" numFmtId="0">
+      <sharedItems count="21">
+        <s v="Great Barrier Reef"/>
+        <s v="Perth"/>
+        <s v="Santiago"/>
+        <s v="London"/>
+        <s v="Bognor"/>
+        <s v="Lyon"/>
+        <s v="Paris - Euro Disney"/>
+        <s v="Nice"/>
+        <s v="Toulouse"/>
+        <s v="Nimes"/>
+        <s v="Black Forest"/>
+        <s v="Berlin"/>
+        <s v="Lima"/>
+        <s v="Riyadh"/>
+        <s v="Barcelona"/>
+        <s v="Nerja"/>
+        <s v="Malaga"/>
+        <s v="Seville"/>
+        <s v="Madrid"/>
+        <s v="Granada"/>
+        <s v="Port of Spain"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="No of Days" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="32"/>
+    </cacheField>
+    <cacheField name="Travel Method" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Plane"/>
+        <s v="Train"/>
+        <s v="Coach"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Price" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="1259" count="24">
+        <n v="750"/>
+        <n v="985"/>
+        <n v="1259"/>
+        <n v="69"/>
+        <n v="12"/>
+        <n v="399"/>
+        <n v="269"/>
+        <n v="125"/>
+        <n v="289"/>
+        <n v="256"/>
+        <n v="287"/>
+        <n v="975"/>
+        <n v="995"/>
+        <n v="219"/>
+        <n v="198"/>
+        <n v="234"/>
+        <n v="288"/>
+        <n v="199"/>
+        <n v="177"/>
+        <n v="301"/>
+        <n v="299"/>
+        <n v="277"/>
+        <n v="345"/>
+        <n v="885"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Holiday ID" numFmtId="0">
+      <sharedItems count="27">
+        <s v="I990AUS"/>
+        <s v="AUS112J"/>
+        <s v="CH266H"/>
+        <s v="I456UK"/>
+        <s v="BG726H"/>
+        <s v="A7995FR"/>
+        <s v="TH789FR"/>
+        <s v="TH788FR"/>
+        <s v="I7897FR"/>
+        <s v="SG7637L"/>
+        <s v="FR5625J"/>
+        <s v="A111G"/>
+        <s v="BR6736G"/>
+        <s v="PG7836G"/>
+        <s v="KSA8987"/>
+        <s v="I6675SP"/>
+        <s v="TH990ESP"/>
+        <s v="A776ESP"/>
+        <s v="NM9876Y"/>
+        <s v="TH8956SP"/>
+        <s v="AJ9836L"/>
+        <s v="GG9836P"/>
+        <s v="PL8726P"/>
+        <s v="SV767HH"/>
+        <s v="WE6735L"/>
+        <s v="GR7878G"/>
+        <s v="TT67624G"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="28">
+  <r>
+    <s v="Australia"/>
+    <x v="0"/>
+    <n v="32"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Australia"/>
+    <x v="1"/>
+    <n v="28"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Chile"/>
+    <x v="2"/>
+    <n v="21"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="England"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="England"/>
+    <x v="4"/>
+    <n v="1"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="France"/>
+    <x v="5"/>
+    <n v="14"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="France"/>
+    <x v="6"/>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="France"/>
+    <x v="6"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="France"/>
+    <x v="7"/>
+    <n v="7"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="France"/>
+    <x v="8"/>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="France"/>
+    <x v="9"/>
+    <n v="7"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Germany"/>
+    <x v="10"/>
+    <n v="4"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Germany"/>
+    <x v="11"/>
+    <n v="7"/>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="Peru"/>
+    <x v="12"/>
+    <n v="21"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <s v="Saudi Arabia"/>
+    <x v="13"/>
+    <n v="14"/>
+    <x v="0"/>
+    <x v="12"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="14"/>
+    <n v="4"/>
+    <x v="1"/>
+    <x v="13"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="15"/>
+    <n v="6"/>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="16"/>
+    <n v="16"/>
+    <x v="0"/>
+    <x v="15"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="17"/>
+    <n v="14"/>
+    <x v="0"/>
+    <x v="16"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="17"/>
+    <n v="10"/>
+    <x v="0"/>
+    <x v="17"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="14"/>
+    <n v="8"/>
+    <x v="0"/>
+    <x v="18"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="14"/>
+    <n v="7"/>
+    <x v="2"/>
+    <x v="17"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="16"/>
+    <n v="14"/>
+    <x v="0"/>
+    <x v="19"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="14"/>
+    <n v="4"/>
+    <x v="1"/>
+    <x v="13"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="17"/>
+    <n v="14"/>
+    <x v="1"/>
+    <x v="20"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="18"/>
+    <n v="8"/>
+    <x v="0"/>
+    <x v="21"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <s v="Spain"/>
+    <x v="19"/>
+    <n v="10"/>
+    <x v="0"/>
+    <x v="22"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <s v="Trinidad"/>
+    <x v="20"/>
+    <n v="14"/>
+    <x v="0"/>
+    <x v="23"/>
+    <x v="26"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C0E41333-8118-9244-8AEF-8C183677BC9A}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="22">
+        <item h="1" x="14"/>
+        <item h="1" x="11"/>
+        <item h="1" x="10"/>
+        <item h="1" x="4"/>
+        <item h="1" x="19"/>
+        <item h="1" x="0"/>
+        <item h="1" x="12"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="18"/>
+        <item h="1" x="16"/>
+        <item h="1" x="15"/>
+        <item h="1" x="7"/>
+        <item h="1" x="9"/>
+        <item h="1" x="6"/>
+        <item h="1" x="1"/>
+        <item h="1" x="20"/>
+        <item h="1" x="13"/>
+        <item x="2"/>
+        <item x="17"/>
+        <item h="1" x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0">
+      <items count="25">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="18"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="21"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="8"/>
+        <item x="20"/>
+        <item x="19"/>
+        <item x="22"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="23"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="28">
+        <item x="11"/>
+        <item x="17"/>
+        <item x="5"/>
+        <item x="20"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item x="21"/>
+        <item x="25"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item x="18"/>
+        <item x="13"/>
+        <item x="22"/>
+        <item x="9"/>
+        <item x="23"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="19"/>
+        <item x="16"/>
+        <item x="26"/>
+        <item x="24"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of Price" fld="4" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -368,7 +891,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,9 +923,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,6 +975,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -609,22 +1168,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66477F6-CE4E-7449-8DC9-E65311DBA9F0}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="24" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="10">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="10">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="10">
+        <v>582</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +1275,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -642,7 +1283,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -662,7 +1303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -682,7 +1323,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -702,7 +1343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>48</v>
       </c>
@@ -722,7 +1363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -742,7 +1383,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -762,7 +1403,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -782,7 +1423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -802,7 +1443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -822,7 +1463,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -842,7 +1483,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -862,7 +1503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -882,7 +1523,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -902,7 +1543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -922,7 +1563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
@@ -942,7 +1583,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -962,7 +1603,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
@@ -982,7 +1623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +1643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
@@ -1022,7 +1663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1042,7 +1683,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +1723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
@@ -1102,7 +1743,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
@@ -1122,7 +1763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
@@ -1142,7 +1783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
@@ -1162,7 +1803,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
@@ -1182,7 +1823,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1202,7 +1843,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>51</v>
       </c>
@@ -1223,7 +1864,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:F42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F42">
     <sortCondition ref="A27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>